<commit_message>
User register and search for a product
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/TestData.xlsx
+++ b/src/test/java/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NopCommerce\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A79F95A-BBE2-47BA-9988-31B644580B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E233B174-F64D-4130-8083-86BB43560408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00D4E611-3088-489F-B746-9D08D6712492}"/>
   </bookViews>
@@ -35,9 +35,56 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>singh</t>
+  </si>
+  <si>
+    <t>ravinder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User register details </t>
+  </si>
+  <si>
+    <t>Gender:</t>
+  </si>
+  <si>
+    <t>First name:</t>
+  </si>
+  <si>
+    <t>Last name:</t>
+  </si>
+  <si>
+    <t>Password:</t>
+  </si>
+  <si>
+    <t>qwerty123</t>
+  </si>
+  <si>
+    <t>Product to search</t>
+  </si>
+  <si>
+    <t>Product name:</t>
+  </si>
+  <si>
+    <t>Apple MacBook</t>
+  </si>
+  <si>
+    <t>Apple MacBook Pro 13-inch</t>
+  </si>
+  <si>
+    <t>Product searched verify:</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,13 +92,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -66,8 +127,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,12 +444,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1481797-CD55-419D-B18D-667C91C2DF7D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.5546875" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Register user and add product to wishlist
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/TestData.xlsx
+++ b/src/test/java/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NopCommerce\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E233B174-F64D-4130-8083-86BB43560408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DFF16C-8AD5-4F49-8D77-235AA07210DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00D4E611-3088-489F-B746-9D08D6712492}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>male</t>
   </si>
@@ -78,6 +78,42 @@
   </si>
   <si>
     <t>Product searched verify:</t>
+  </si>
+  <si>
+    <t>Computers</t>
+  </si>
+  <si>
+    <t>Nav menu options</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Desktops </t>
+  </si>
+  <si>
+    <t>Digital Storm VANQUISH 3 Custom Performance PC</t>
+  </si>
+  <si>
+    <t>Destop product to add:</t>
+  </si>
+  <si>
+    <t>Computes sub category option:</t>
+  </si>
+  <si>
+    <t>Nav menu option:</t>
+  </si>
+  <si>
+    <t>Checkout details</t>
+  </si>
+  <si>
+    <t>City:</t>
+  </si>
+  <si>
+    <t>Mohali</t>
+  </si>
+  <si>
+    <t>Address 1:</t>
+  </si>
+  <si>
+    <t>Sector 71</t>
   </si>
 </sst>
 </file>
@@ -127,9 +163,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,18 +485,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1481797-CD55-419D-B18D-667C91C2DF7D}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="27.5546875" customWidth="1"/>
-    <col min="3" max="3" width="23.21875" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -464,30 +506,30 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -497,19 +539,67 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>